<commit_message>
Bonnie/prod bug 65 (#17)
* 提品匯入範例，「商品完整說明」欄位名稱下方加上文字提示「請使用HTML語法執行文字排版」

* fix
</commit_message>
<xml_diff>
--- a/public/files/提品匯入範例.xlsx
+++ b/public/files/提品匯入範例.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f4564\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\cec-scm-mgt\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B54C80-C0A5-48AD-892B-969F4415639F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170DE9FA-EA68-4AC3-8C5B-C5011EDBD182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2498" yWindow="1575" windowWidth="16904" windowHeight="10185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="功能說明" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
@@ -4954,10 +4952,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>請輸入商品完整說明文字</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>請輸入產品成份及食品添加物 文字</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -5170,6 +5164,10 @@
   </si>
   <si>
     <t>請輸入商品高度，以cm為單位，請輸入數字</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>請輸入商品完整說明文字（請使用HTML語法執行文字排版）</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -5799,7 +5797,7 @@
     </row>
     <row r="4" spans="1:12" ht="176.25" customHeight="1" thickBot="1">
       <c r="A4" s="24" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -5824,7 +5822,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BD30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -5942,7 +5942,7 @@
         <v>1064</v>
       </c>
       <c r="AD1" s="21" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="AE1" s="21" t="s">
         <v>1065</v>
@@ -5963,7 +5963,7 @@
         <v>1576</v>
       </c>
       <c r="AK1" s="21" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="AL1" s="21" t="s">
         <v>1597</v>
@@ -5978,10 +5978,10 @@
         <v>1600</v>
       </c>
       <c r="AP1" s="21" t="s">
+        <v>1638</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
         <v>1639</v>
-      </c>
-      <c r="AQ1" s="21" t="s">
-        <v>1640</v>
       </c>
       <c r="AR1" s="21" t="s">
         <v>1601</v>
@@ -5993,7 +5993,7 @@
         <v>1603</v>
       </c>
       <c r="AU1" s="21" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="AV1" s="21" t="s">
         <v>1604</v>
@@ -6195,172 +6195,172 @@
     </row>
     <row r="3" spans="1:56" s="16" customFormat="1" ht="210" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="16" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>1619</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="C3" s="16" t="s">
         <v>1620</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>1621</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
+        <v>1641</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>1622</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>1642</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>1623</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="I3" s="16" t="s">
+        <v>1624</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>1625</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>1626</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>1661</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>1662</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>1663</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>1627</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>1628</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>1629</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>1630</v>
+      </c>
+      <c r="S3" s="16" t="s">
         <v>1643</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>1624</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>1625</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>1626</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>1627</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>1662</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>1663</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>1664</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>1628</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>1629</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>1630</v>
-      </c>
-      <c r="R3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>1631</v>
       </c>
-      <c r="S3" s="16" t="s">
-        <v>1644</v>
-      </c>
-      <c r="T3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>1632</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="V3" s="16" t="s">
         <v>1633</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>1634</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>1635</v>
-      </c>
-      <c r="X3" s="16" t="s">
-        <v>1636</v>
       </c>
       <c r="Y3" s="16" t="s">
         <v>1614</v>
       </c>
       <c r="Z3" s="16" t="s">
+        <v>1659</v>
+      </c>
+      <c r="AA3" s="16" t="s">
         <v>1660</v>
       </c>
-      <c r="AA3" s="16" t="s">
-        <v>1661</v>
-      </c>
       <c r="AB3" s="16" t="s">
+        <v>1664</v>
+      </c>
+      <c r="AC3" s="16" t="s">
         <v>1615</v>
       </c>
-      <c r="AC3" s="16" t="s">
+      <c r="AD3" s="16" t="s">
         <v>1616</v>
       </c>
-      <c r="AD3" s="16" t="s">
+      <c r="AE3" s="16" t="s">
         <v>1617</v>
       </c>
-      <c r="AE3" s="16" t="s">
-        <v>1618</v>
-      </c>
       <c r="AF3" s="16" t="s">
+        <v>1644</v>
+      </c>
+      <c r="AG3" s="16" t="s">
+        <v>1646</v>
+      </c>
+      <c r="AH3" s="16" t="s">
         <v>1645</v>
       </c>
-      <c r="AG3" s="16" t="s">
+      <c r="AI3" s="16" t="s">
         <v>1647</v>
       </c>
-      <c r="AH3" s="16" t="s">
-        <v>1646</v>
-      </c>
-      <c r="AI3" s="16" t="s">
+      <c r="AJ3" s="16" t="s">
         <v>1648</v>
       </c>
-      <c r="AJ3" s="16" t="s">
+      <c r="AK3" s="16" t="s">
         <v>1649</v>
       </c>
-      <c r="AK3" s="16" t="s">
+      <c r="AL3" s="16" t="s">
         <v>1650</v>
       </c>
-      <c r="AL3" s="16" t="s">
-        <v>1651</v>
-      </c>
       <c r="AM3" s="16" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="AN3" s="16" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="AO3" s="16" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="AP3" s="16" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="AQ3" s="16" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="AR3" s="16" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="AS3" s="16" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="AT3" s="16" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="AU3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="AV3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="AW3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="AX3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="AY3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="AZ3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="BA3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="BB3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="BC3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="BD3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="4" spans="1:56" ht="16.5" customHeight="1"/>
@@ -6443,7 +6443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BC30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -6578,7 +6580,7 @@
         <v>1070</v>
       </c>
       <c r="AJ1" s="21" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="AK1" s="21" t="s">
         <v>27</v>
@@ -6593,10 +6595,10 @@
         <v>30</v>
       </c>
       <c r="AO1" s="21" t="s">
+        <v>1638</v>
+      </c>
+      <c r="AP1" s="21" t="s">
         <v>1639</v>
-      </c>
-      <c r="AP1" s="21" t="s">
-        <v>1640</v>
       </c>
       <c r="AQ1" s="21" t="s">
         <v>31</v>
@@ -6819,13 +6821,13 @@
         <v>1580</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>1581</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>1582</v>
@@ -6840,13 +6842,13 @@
         <v>1585</v>
       </c>
       <c r="L3" s="16" t="s">
+        <v>1661</v>
+      </c>
+      <c r="M3" s="16" t="s">
         <v>1662</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>1663</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>1664</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>1586</v>
@@ -6882,94 +6884,94 @@
         <v>1596</v>
       </c>
       <c r="Z3" s="16" t="s">
+        <v>1659</v>
+      </c>
+      <c r="AA3" s="16" t="s">
         <v>1660</v>
       </c>
-      <c r="AA3" s="16" t="s">
-        <v>1661</v>
-      </c>
       <c r="AB3" s="16" t="s">
-        <v>1615</v>
+        <v>1664</v>
       </c>
       <c r="AC3" s="16" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AD3" s="16" t="s">
         <v>1652</v>
       </c>
-      <c r="AD3" s="16" t="s">
+      <c r="AE3" s="16" t="s">
         <v>1653</v>
       </c>
-      <c r="AE3" s="16" t="s">
+      <c r="AF3" s="16" t="s">
         <v>1654</v>
       </c>
-      <c r="AF3" s="16" t="s">
+      <c r="AG3" s="16" t="s">
         <v>1655</v>
       </c>
-      <c r="AG3" s="16" t="s">
+      <c r="AH3" s="16" t="s">
+        <v>1647</v>
+      </c>
+      <c r="AI3" s="16" t="s">
         <v>1656</v>
       </c>
-      <c r="AH3" s="16" t="s">
-        <v>1648</v>
-      </c>
-      <c r="AI3" s="16" t="s">
+      <c r="AJ3" s="16" t="s">
+        <v>1649</v>
+      </c>
+      <c r="AK3" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="AL3" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="AM3" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="AN3" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="AO3" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="AP3" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="AQ3" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="AR3" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="AS3" s="16" t="s">
+        <v>1650</v>
+      </c>
+      <c r="AT3" s="25" t="s">
         <v>1657</v>
       </c>
-      <c r="AJ3" s="16" t="s">
-        <v>1650</v>
-      </c>
-      <c r="AK3" s="16" t="s">
-        <v>1651</v>
-      </c>
-      <c r="AL3" s="16" t="s">
-        <v>1651</v>
-      </c>
-      <c r="AM3" s="16" t="s">
-        <v>1651</v>
-      </c>
-      <c r="AN3" s="16" t="s">
-        <v>1651</v>
-      </c>
-      <c r="AO3" s="16" t="s">
-        <v>1651</v>
-      </c>
-      <c r="AP3" s="16" t="s">
-        <v>1651</v>
-      </c>
-      <c r="AQ3" s="16" t="s">
-        <v>1651</v>
-      </c>
-      <c r="AR3" s="16" t="s">
-        <v>1651</v>
-      </c>
-      <c r="AS3" s="16" t="s">
-        <v>1651</v>
-      </c>
-      <c r="AT3" s="25" t="s">
-        <v>1658</v>
-      </c>
       <c r="AU3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="AV3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="AW3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="AX3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="AY3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="AZ3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="BA3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="BB3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="BC3" s="25" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="4" spans="1:55" ht="16.5" customHeight="1"/>

</xml_diff>